<commit_message>
Updated DP2_assignment03b to v2
</commit_message>
<xml_diff>
--- a/DP2_assignment03a/doc/NffgServiceAPI.xlsx
+++ b/DP2_assignment03a/doc/NffgServiceAPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="53">
   <si>
     <t>Resource</t>
   </si>
@@ -131,9 +131,6 @@
     <t>CREATED - new nffg loaded</t>
   </si>
   <si>
-    <t>BAD REQUEST - nffg not loaded</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -149,14 +146,50 @@
     <t>BAD REQUEST - nffg not deleted</t>
   </si>
   <si>
-    <t>??? La verifica ???</t>
+    <t>CREATED - new policy loaded</t>
+  </si>
+  <si>
+    <t>BAD REQUEST - policy not loaded</t>
+  </si>
+  <si>
+    <t>RESET CONTENT - policies deleted</t>
+  </si>
+  <si>
+    <t>policies/verification</t>
+  </si>
+  <si>
+    <t>names: stringList</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>names:stringList</t>
+  </si>
+  <si>
+    <t>OK - policies verification results are inside response</t>
+  </si>
+  <si>
+    <t>OK - posted policies verification results are inside response</t>
+  </si>
+  <si>
+    <t>BAD REQUEST - policies not verified</t>
+  </si>
+  <si>
+    <t>NOT FOUND - policies not found</t>
+  </si>
+  <si>
+    <t>namesType</t>
+  </si>
+  <si>
+    <t>NOT FOUND - nffs not deleted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,16 +197,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -181,16 +226,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valore valido" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -502,55 +567,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -567,70 +647,70 @@
         <v>14</v>
       </c>
       <c r="F3">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -639,56 +719,56 @@
         <v>400</v>
       </c>
       <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>205</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>205</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>400</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1">
+        <v>404</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -711,7 +791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -734,12 +814,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -754,15 +834,15 @@
         <v>205</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -777,30 +857,34 @@
         <v>400</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>200</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>404</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -810,16 +894,19 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
       <c r="F14">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -827,17 +914,14 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
       <c r="F15">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -847,16 +931,19 @@
       <c r="C16" t="s">
         <v>8</v>
       </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
       <c r="F16">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -864,14 +951,11 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
       <c r="F17">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -888,15 +972,15 @@
         <v>19</v>
       </c>
       <c r="F18">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -905,41 +989,233 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>204</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F19">
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1">
+        <v>201</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1">
+        <v>400</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1">
+        <v>205</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1">
+        <v>205</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24">
         <v>200</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20">
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
         <v>404</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26">
+        <v>200</v>
+      </c>
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="1">
+        <v>400</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="1">
+        <v>200</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="1">
+        <v>404</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
NffgService demo ver 0.01
</commit_message>
<xml_diff>
--- a/DP2_assignment03a/doc/NffgServiceAPI.xlsx
+++ b/DP2_assignment03a/doc/NffgServiceAPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
   <si>
     <t>Resource</t>
   </si>
@@ -98,27 +98,9 @@
     <t>PUT</t>
   </si>
   <si>
-    <t>NOT FOUND - policies not found</t>
-  </si>
-  <si>
     <t>deletePolicies: boolean</t>
   </si>
   <si>
-    <t>CREATED - new policies loaded</t>
-  </si>
-  <si>
-    <t>BAD REQUEST - nffg not deleted (e.g. policies not deleted)</t>
-  </si>
-  <si>
-    <t>BAD REQUEST - policies not loaded (e.g. missing nffg)</t>
-  </si>
-  <si>
-    <t>policy</t>
-  </si>
-  <si>
-    <t>BAD REQUEST - policies not verified (e.g. missing nffg)</t>
-  </si>
-  <si>
     <t>namedEntities: to verify policy's names</t>
   </si>
   <si>
@@ -128,15 +110,6 @@
     <t>policies/verifier</t>
   </si>
   <si>
-    <t>PARTIAL CONTENT - policy updated (verification result and update time)</t>
-  </si>
-  <si>
-    <t>BAD REQUEST - policy not updated (e.g. missing nffg)</t>
-  </si>
-  <si>
-    <t>BAD REQUEST - nffgs not loaded</t>
-  </si>
-  <si>
     <t>OK - policies verified (results are inside policies)</t>
   </si>
   <si>
@@ -150,6 +123,33 @@
   </si>
   <si>
     <t>NO CONTENT - policies deleted</t>
+  </si>
+  <si>
+    <t>FORBIDDEN - nffg has policies (only if query param false)</t>
+  </si>
+  <si>
+    <t>NO CONTENT - new policies loaded</t>
+  </si>
+  <si>
+    <t>NO CONTENT - policy deleted</t>
+  </si>
+  <si>
+    <t>OK - policy updated (verification result and update time)</t>
+  </si>
+  <si>
+    <t>FORBIDDEN - policy not updated (e.g. missing nffg)</t>
+  </si>
+  <si>
+    <t>FORBIDDEN - policies not verified (e.g. missing policy)</t>
+  </si>
+  <si>
+    <t>FORBIDDEN - nffgs not loaded (e.g. already loaded nffg)</t>
+  </si>
+  <si>
+    <t>FORBIDDEN - policies not loaded (e.g. missing nffg or already loaded policy)</t>
+  </si>
+  <si>
+    <t>FORBIDDEN - policies not verified (e.g. missing nffg)</t>
   </si>
 </sst>
 </file>
@@ -535,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -661,10 +661,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="1">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -684,10 +684,10 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -753,10 +753,10 @@
         <v>8</v>
       </c>
       <c r="F9">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -775,11 +775,11 @@
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10">
-        <v>400</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
+      <c r="F10" s="1">
+        <v>403</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -866,13 +866,13 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1">
         <v>201</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -892,10 +892,10 @@
         <v>8</v>
       </c>
       <c r="F15" s="1">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -915,10 +915,10 @@
         <v>8</v>
       </c>
       <c r="F16" s="1">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>200</v>
@@ -978,16 +978,16 @@
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1001,16 +1001,16 @@
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>8</v>
@@ -1037,77 +1037,77 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22">
-        <v>200</v>
-      </c>
-      <c r="G22" t="s">
-        <v>37</v>
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1">
+        <v>204</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1">
+        <v>404</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1">
-        <v>400</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24">
         <v>200</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>32</v>
+      <c r="G24" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -1116,39 +1116,62 @@
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="1">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1">
+        <v>403</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>